<commit_message>
Added Test Case File
</commit_message>
<xml_diff>
--- a/src/Resources/TestCase.xlsx
+++ b/src/Resources/TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samir\eclipse-workspace\ATMFramework\src\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762B978A-A1B0-4571-AC1F-253FC9582991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F72A824-2FCA-4C1C-941C-4BA7DB2260CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>SNO</t>
   </si>
@@ -42,56 +42,26 @@
     <t>TEST DATA</t>
   </si>
   <si>
-    <t>CLICK</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>sample1</t>
   </si>
   <si>
-    <t>sample2</t>
-  </si>
-  <si>
-    <t>sample3</t>
-  </si>
-  <si>
-    <t>SENDKEYS</t>
-  </si>
-  <si>
-    <t>xpath=//*[text()="Samir1"]</t>
-  </si>
-  <si>
-    <t>xpath=//*[text()="Samir2"]</t>
-  </si>
-  <si>
-    <t>sampleData1</t>
-  </si>
-  <si>
-    <t>sampleData2</t>
-  </si>
-  <si>
-    <t>TAPPING</t>
-  </si>
-  <si>
-    <t>xpath=//*[text()="Samir3"]</t>
-  </si>
-  <si>
-    <t>sampleData3</t>
+    <t>NavigateTo</t>
+  </si>
+  <si>
+    <t>https://www.google.com/</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +78,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,20 +167,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,18 +462,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -514,57 +495,26 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{556FD41B-D21B-40AD-ABCA-A846724DEDB0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lakshmi changes updated for samir review
</commit_message>
<xml_diff>
--- a/src/Resources/TestCase.xlsx
+++ b/src/Resources/TestCase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samir\eclipse-workspace\ATMFramework\src\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GITRepo\Selenium\SeleniumScripts\ATMFrm1\src\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F72A824-2FCA-4C1C-941C-4BA7DB2260CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE3265E-743B-48BA-94F0-E8DB1A2744E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>SNO</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>https://www.bing.com/</t>
+  </si>
+  <si>
+    <t>explicitwait</t>
   </si>
 </sst>
 </file>
@@ -172,7 +184,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
@@ -180,6 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -462,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,10 +523,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{556FD41B-D21B-40AD-ABCA-A846724DEDB0}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{391536F9-2D3C-45D2-9DE7-61233B1547B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated with testcase .xls
</commit_message>
<xml_diff>
--- a/src/Resources/TestCase.xlsx
+++ b/src/Resources/TestCase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GITRepo\Selenium\SeleniumScripts\Framework\ATMFrm1\src\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GITRepo\Selenium\SeleniumScripts\ATM_01\src\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652D9C8A-9FE2-42E7-8761-A3864F7F5057}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE63D5D-45EC-476F-BC13-A24CE537C322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>SNO</t>
   </si>
@@ -45,40 +45,115 @@
     <t>1</t>
   </si>
   <si>
-    <t>sample1</t>
-  </si>
-  <si>
     <t>NavigateTo</t>
   </si>
   <si>
-    <t>https://www.google.com/</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>sample2</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>https://www.bing.com/</t>
-  </si>
-  <si>
     <t>explicitwait</t>
   </si>
   <si>
-    <t>Sample3</t>
+    <t>3</t>
   </si>
   <si>
     <t>implicitwait</t>
   </si>
   <si>
-    <t>https://www.guru99.com/implicit-explicit-waits-selenium.html</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>LaunchURL</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/automation-practice-form</t>
+  </si>
+  <si>
+    <t>ThinkTime</t>
+  </si>
+  <si>
+    <t>Implicitwait</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Enter Firstname</t>
+  </si>
+  <si>
+    <t>SendKeys</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Enter LastName</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Enter email</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Gender Selection</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Enter Mobile Number</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>//input[@id="firstName"]</t>
+  </si>
+  <si>
+    <t>//input[@id="lastName"]</t>
+  </si>
+  <si>
+    <t>//input[@id="userEmail"]</t>
+  </si>
+  <si>
+    <t>//input[@placeholder="Mobile Number"]</t>
+  </si>
+  <si>
+    <t>//label[@for="gender-radio-1"]</t>
+  </si>
+  <si>
+    <t>Lakshmi1</t>
+  </si>
+  <si>
+    <t>Narayanan1</t>
+  </si>
+  <si>
+    <t>lakshmi1137@gmail.com</t>
+  </si>
+  <si>
+    <t>9940501761</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>//button[@class="btn btn-primary"]</t>
   </si>
 </sst>
 </file>
@@ -196,15 +271,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -487,18 +582,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B10" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.6640625" customWidth="1"/>
+    <col min="5" max="5" width="53.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -523,58 +618,178 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="D3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>16</v>
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{556FD41B-D21B-40AD-ABCA-A846724DEDB0}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{391536F9-2D3C-45D2-9DE7-61233B1547B9}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{77F7DC7A-8815-4EAC-BA35-125C2817E7C7}"/>
+    <hyperlink ref="E6" r:id="rId1" display="https://www.guru99.com/implicit-explicit-waits-selenium.html" xr:uid="{704B10C2-EC30-405F-8A78-25EAFB20A54F}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{6B160C9B-E517-4246-AD84-345FAC86E6CD}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{FF462B4E-77D0-4EFF-ACAB-9462B644B1C1}"/>
+    <hyperlink ref="E5" r:id="rId4" display="lakshmi137@gmail.com" xr:uid="{07D55FAE-3F88-4C29-B233-5A9467767081}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>